<commit_message>
Pulito codice e aggiunto grafico e albo d'oro
</commit_message>
<xml_diff>
--- a/FsStats.xlsx
+++ b/FsStats.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paolo\Desktop\Streamlit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paolo\Desktop\Git Project\fanta-dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43899545-11B4-4932-88B3-5E057D66B478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{346F30A4-892C-4E7B-801B-1712345BF76A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11820" yWindow="750" windowWidth="14085" windowHeight="10680" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="16-17" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="21-22" sheetId="6" r:id="rId6"/>
     <sheet name="22-23" sheetId="7" r:id="rId7"/>
     <sheet name="23-24" sheetId="8" r:id="rId8"/>
+    <sheet name="Albo" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="41">
   <si>
     <t>Pos</t>
   </si>
@@ -109,6 +110,60 @@
   </si>
   <si>
     <t>Los Polpos</t>
+  </si>
+  <si>
+    <t>Fantastrambino</t>
+  </si>
+  <si>
+    <t>Fs Cup</t>
+  </si>
+  <si>
+    <t>Fs SuperCup</t>
+  </si>
+  <si>
+    <t>16-17</t>
+  </si>
+  <si>
+    <t>Lirlanda</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>17-18</t>
+  </si>
+  <si>
+    <t>18-19</t>
+  </si>
+  <si>
+    <t>19-20</t>
+  </si>
+  <si>
+    <t>20-21</t>
+  </si>
+  <si>
+    <t>21-22</t>
+  </si>
+  <si>
+    <t>22-23</t>
+  </si>
+  <si>
+    <t>23-24</t>
+  </si>
+  <si>
+    <t>Anno</t>
+  </si>
+  <si>
+    <t>Lirlanda, SS Egli Tare 2016</t>
+  </si>
+  <si>
+    <t>Retrocessioni</t>
+  </si>
+  <si>
+    <t>FC Dragoes (rit)</t>
+  </si>
+  <si>
+    <t>AC Gallianese</t>
   </si>
 </sst>
 </file>
@@ -150,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -158,6 +213,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -494,7 +550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
@@ -3751,4 +3807,180 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1F0B8A8-F904-4DC7-B10B-D7106C4A96DE}">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D14" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Aggiunto boxplot e medie
</commit_message>
<xml_diff>
--- a/FsStats.xlsx
+++ b/FsStats.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paolo\Desktop\Git Project\fanta-dashboard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paolo\Desktop\Nuova cartella\Git Project\fanta-dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{346F30A4-892C-4E7B-801B-1712345BF76A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE30D55-2BEE-41C6-87F0-6EF66E819D49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11820" yWindow="750" windowWidth="14085" windowHeight="10680" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="16-17" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="22-23" sheetId="7" r:id="rId7"/>
     <sheet name="23-24" sheetId="8" r:id="rId8"/>
     <sheet name="Albo" sheetId="9" r:id="rId9"/>
+    <sheet name="Riassunto" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="46">
   <si>
     <t>Pos</t>
   </si>
@@ -124,9 +125,6 @@
     <t>16-17</t>
   </si>
   <si>
-    <t>Lirlanda</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -154,9 +152,6 @@
     <t>Anno</t>
   </si>
   <si>
-    <t>Lirlanda, SS Egli Tare 2016</t>
-  </si>
-  <si>
     <t>Retrocessioni</t>
   </si>
   <si>
@@ -164,13 +159,34 @@
   </si>
   <si>
     <t>AC Gallianese</t>
+  </si>
+  <si>
+    <t>Calendario</t>
+  </si>
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>Rose</t>
+  </si>
+  <si>
+    <t>Dettagli</t>
+  </si>
+  <si>
+    <t>Abbiamo le formazioni,  è recuperabile con un po' di lavoro</t>
+  </si>
+  <si>
+    <t>Lirlanda FC, SS Egli Tare 2016</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,6 +199,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -213,7 +237,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -551,7 +575,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="U29" sqref="U29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -905,6 +929,142 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D5A1476-2592-499C-9341-0D6372419C94}">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3811,22 +3971,22 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1F0B8A8-F904-4DC7-B10B-D7106C4A96DE}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
         <v>23</v>
@@ -3838,63 +3998,63 @@
         <v>25</v>
       </c>
       <c r="E1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>26</v>
       </c>
       <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
         <v>27</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>28</v>
-      </c>
-      <c r="D2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>29</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
       </c>
       <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
         <v>27</v>
       </c>
-      <c r="E4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
@@ -3903,15 +4063,15 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
         <v>16</v>
@@ -3923,12 +4083,12 @@
         <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
@@ -3940,29 +4100,29 @@
         <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
         <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
         <v>22</v>
@@ -3974,11 +4134,11 @@
         <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D14" s="3"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F14" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>